<commit_message>
Support First And Second Half 1325 Calculations
</commit_message>
<xml_diff>
--- a/TaxMaster.Infra/Assets/1325Form.xlsx
+++ b/TaxMaster.Infra/Assets/1325Form.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ybenharosh\source\repos\TaxMaster\TaxMaster.Infra\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149103A6-B922-4A61-8DE3-31DA313CAB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C06F160-1969-42FC-B625-7FA8BED44A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2EAC2B80-7C28-4C96-B290-8BE40F8543A1}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2EAC2B80-7C28-4C96-B290-8BE40F8543A1}"/>
   </bookViews>
   <sheets>
     <sheet name="1325" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'1325'!$A$1:$L$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'1325'!$A$1:$L$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1014,8 +1014,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{331D903F-145D-4022-9AB6-9A1FC3AD8457}" name="Table53" displayName="Table53" ref="A4:L14" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
-  <autoFilter ref="A4:L14" xr:uid="{EDDFF828-E11C-4C14-974A-F5FB5050A084}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{331D903F-145D-4022-9AB6-9A1FC3AD8457}" name="Table53" displayName="Table53" ref="A4:L24" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+  <autoFilter ref="A4:L24" xr:uid="{EDDFF828-E11C-4C14-974A-F5FB5050A084}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{10D4D436-818E-4F8E-ACBF-6A12B900601E}" name=" " dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{2F9CBED6-E433-43FA-A017-97779ABA6D45}" name="זיהוי מלא של נייר הערך שנמכר לפי הסדר הכרונולוגי של המכירות" dataDxfId="10"/>
@@ -1351,15 +1351,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C952D2-02CC-494D-825B-79121DB2144F}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18:J18"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.625" style="1" bestFit="1" customWidth="1"/>
@@ -1574,60 +1574,220 @@
       <c r="K13" s="15"/>
       <c r="L13" s="14"/>
     </row>
-    <row r="14" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12">
+    <row r="14" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20">
         <v>10</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D17" s="3"/>
-      <c r="I17" s="32" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="14"/>
+    </row>
+    <row r="15" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="20">
+        <v>11</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="20">
+        <v>12</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="14"/>
+    </row>
+    <row r="17" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="20">
+        <v>13</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="14"/>
+    </row>
+    <row r="18" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="20">
+        <v>14</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="14"/>
+    </row>
+    <row r="19" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="20">
+        <v>15</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="14"/>
+    </row>
+    <row r="20" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20">
+        <v>16</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="14"/>
+    </row>
+    <row r="21" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="20">
         <v>17</v>
       </c>
-      <c r="J17" s="33"/>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="4:11" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D18" s="3"/>
-      <c r="I18" s="34" t="s">
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="14"/>
+    </row>
+    <row r="22" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="20">
         <v>18</v>
       </c>
-      <c r="J18" s="35"/>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D19" s="3"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="I22" s="1" t="s">
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="14"/>
+    </row>
+    <row r="23" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="20">
+        <v>19</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="14"/>
+    </row>
+    <row r="24" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="12">
+        <v>20</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D27" s="3"/>
+      <c r="I27" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="33"/>
+      <c r="K27" s="5"/>
+    </row>
+    <row r="28" spans="1:12" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D28" s="3"/>
+      <c r="I28" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="35"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D29" s="3"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I32" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I28:J28"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="58" orientation="landscape" r:id="rId1"/>

</xml_diff>